<commit_message>
"initial fix to quick convert"
</commit_message>
<xml_diff>
--- a/Blackboard_Quiz_Sample.xlsx
+++ b/Blackboard_Quiz_Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robalvarez/Desktop/EdTech QTI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theof\OneDrive\Desktop\examHelperQTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1D26D9CD-2B66-D542-8D1B-9402C9410F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{91DE55F0-9CD7-4D85-A245-66ADBC6A178C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3420" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-12885" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackboard_Quiz_Sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="28" uniqueCount="18">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="28" uniqueCount="19">
   <si>
     <t>MC</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>correct</t>
+  </si>
+  <si>
+    <t>Corrects</t>
   </si>
 </sst>
 </file>
@@ -942,12 +945,12 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="217" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -973,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -990,7 +993,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -1017,7 +1020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
item bank commmit edits button fix
</commit_message>
<xml_diff>
--- a/Blackboard_Quiz_Sample.xlsx
+++ b/Blackboard_Quiz_Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theof\OneDrive\Desktop\examHelperQTI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanrefugia/Desktop/examHelperQTI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{91DE55F0-9CD7-4D85-A245-66ADBC6A178C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A75BADAC-93AF-FD4A-9E3F-96954DB46FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-12885" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackboard_Quiz_Sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="28" uniqueCount="19">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="168" uniqueCount="19">
   <si>
     <t>MC</t>
   </si>
@@ -942,15 +942,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="217" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:N42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -976,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1087,6 +1087,706 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16">
+        <v>7</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>6</v>
+      </c>
+      <c r="L23" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23">
+        <v>7</v>
+      </c>
+      <c r="N23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="H29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30">
+        <v>6</v>
+      </c>
+      <c r="L30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30">
+        <v>7</v>
+      </c>
+      <c r="N30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="H35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="H36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37" t="s">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37" t="s">
+        <v>3</v>
+      </c>
+      <c r="K37">
+        <v>6</v>
+      </c>
+      <c r="L37" t="s">
+        <v>16</v>
+      </c>
+      <c r="M37">
+        <v>7</v>
+      </c>
+      <c r="N37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix in quick convert sticky header and longer preview
</commit_message>
<xml_diff>
--- a/Blackboard_Quiz_Sample.xlsx
+++ b/Blackboard_Quiz_Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanrefugia/Desktop/examHelperQTI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robalvarez/Desktop/examHelperQTI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A75BADAC-93AF-FD4A-9E3F-96954DB46FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{56589946-809E-1C45-B662-C156F7C228D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="33600" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackboard_Quiz_Sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="168" uniqueCount="19">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="196" uniqueCount="18">
   <si>
     <t>MC</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>correct</t>
-  </si>
-  <si>
-    <t>Corrects</t>
   </si>
 </sst>
 </file>
@@ -942,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:N42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="219" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,7 +990,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -1087,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -1133,7 +1130,7 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -1227,7 +1224,7 @@
         <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1273,7 +1270,7 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -1367,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -1413,7 +1410,7 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G23">
         <v>4</v>
@@ -1507,7 +1504,7 @@
         <v>6</v>
       </c>
       <c r="H28" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1553,7 +1550,7 @@
         <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G30">
         <v>4</v>
@@ -1647,7 +1644,7 @@
         <v>6</v>
       </c>
       <c r="H35" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -1693,7 +1690,7 @@
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G37">
         <v>4</v>
@@ -1787,10 +1784,151 @@
         <v>6</v>
       </c>
       <c r="H42" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="H43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44" t="s">
+        <v>3</v>
+      </c>
+      <c r="K44">
+        <v>6</v>
+      </c>
+      <c r="L44" t="s">
+        <v>16</v>
+      </c>
+      <c r="M44">
+        <v>7</v>
+      </c>
+      <c r="N44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>6</v>
+      </c>
+      <c r="H49" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>